<commit_message>
complete bug fixes and refactors on module 3
</commit_message>
<xml_diff>
--- a/Online Retail Project Modules/Module 2/MGECR1.4/MGECR1.4.2.xlsx
+++ b/Online Retail Project Modules/Module 2/MGECR1.4/MGECR1.4.2.xlsx
@@ -339,7 +339,7 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">) == </t>
+      <t xml:space="preserve">) != </t>
     </r>
     <r>
       <rPr>
@@ -940,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -952,7 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -979,31 +979,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1015,52 +1015,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1105,25 +1105,25 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1135,13 +1135,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1191,15 +1191,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>146923</xdr:rowOff>
+      <xdr:rowOff>96809</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1254414</xdr:colOff>
+      <xdr:colOff>1273464</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>43576</xdr:rowOff>
+      <xdr:rowOff>93689</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1208,8 +1208,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3006725" y="146923"/>
-          <a:ext cx="5829590" cy="668179"/>
+          <a:off x="2987674" y="96809"/>
+          <a:ext cx="5880391" cy="768406"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1227,7 +1227,7 @@
         </a:extLst>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" anchor="ctr">
+        <a:bodyPr wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" anchor="ctr">
           <a:normAutofit fontScale="100000" lnSpcReduction="0"/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -1430,9 +1430,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1512,7 +1512,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1540,10 +1540,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1799,9 +1799,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -2089,7 +2089,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2117,10 +2117,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2379,10 +2379,10 @@
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.9062" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7578" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5547" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.9844" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.17188" style="1" customWidth="1"/>
     <col min="8" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>

</xml_diff>